<commit_message>
Proyecto en minitab agregado
</commit_message>
<xml_diff>
--- a/Datos apilados.xlsx
+++ b/Datos apilados.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estudiante\source\repos\PF_ArquitecturaHardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C45DF61-395A-418E-843F-1040F35406E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4940C566-CC99-47DC-8A03-B4E503696EF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F347E8DB-6CC1-4CDB-9EE9-5D387E5D700C}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos apilados" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Datos apilados'!$A$1:$G$481</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -565,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F283F0A-ACF0-4516-8743-152DD0001CAF}">
   <dimension ref="A1:G481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A443" zoomScale="54" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q461" sqref="Q461"/>
+    <sheetView tabSelected="1" topLeftCell="A390" zoomScale="92" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>